<commit_message>
add allure reports and Application TCs
</commit_message>
<xml_diff>
--- a/createdRecords.xlsx
+++ b/createdRecords.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -454,15 +454,175 @@
         <v>DE-TIMS-100694</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>DE-TIMS-100706</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>DE-TIMS-100716</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A12"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Application ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>A153507</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>A153508</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>A153541</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>A153540</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>A153542</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>A153543</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>A153547</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>A153548</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>A153549</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>A153550</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>A153562</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>A153564</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>A153565</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>A153566</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>A153567</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>A153574</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>A153575</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>A153578</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>A153579</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>A153582</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>A153583</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>A153584</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>A153585</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>A153586</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>A153588</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>A153589</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A27"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -471,57 +631,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Application ID</v>
+        <v>Project ID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>A153507</v>
+        <v>P-609807</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>A153508</v>
+        <v>P-609814</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>A153541</v>
+        <v>P-609815</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>A153540</v>
+        <v>P-609820</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>A153542</v>
+        <v>P-609829</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>A153543</v>
+        <v>DE-TIMS-100104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>A153547</v>
+        <v>P-609832</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>A153548</v>
+        <v>P-609833</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>A153549</v>
+        <v>P-609836</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>A153550</v>
+        <v>P-609837</v>
       </c>
     </row>
   </sheetData>
@@ -530,44 +690,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:A11"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Project ID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>P-609807</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>P-609814</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>P-609815</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>P-609820</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Allure report to add-regression-TCs
</commit_message>
<xml_diff>
--- a/createdRecords.xlsx
+++ b/createdRecords.xlsx
@@ -6,6 +6,9 @@
     <sheet name="Site" sheetId="1" r:id="rId1"/>
     <sheet name="Application" sheetId="2" r:id="rId2"/>
     <sheet name="Project" sheetId="3" r:id="rId3"/>
+    <sheet name="Request" sheetId="4" r:id="rId4"/>
+    <sheet name="Lease" sheetId="5" r:id="rId5"/>
+    <sheet name="Candidate" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -409,72 +412,17 @@
         <v>Site ID</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>DE-TIMS-100661</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>DE-TIMS-100676</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>DE-TIMS-100104</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>DE-TIMS-100104</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>DE-TIMS-100104</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>DE-TIMS-100678</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>DE-TIMS-100686</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>DE-TIMS-100690</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>DE-TIMS-100694</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>DE-TIMS-100706</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>DE-TIMS-100716</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -486,145 +434,250 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>A153507</v>
+        <v>A227169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>A153508</v>
+        <v>A227168</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>A153541</v>
+        <v>A227170</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>A153540</v>
+        <v>A227171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>A153542</v>
+        <v>A227187</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>A153543</v>
+        <v>A227188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>A153547</v>
+        <v>A227189</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>A153548</v>
+        <v>A227190</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>A153549</v>
+        <v>A227195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>A153550</v>
+        <v>A227196</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>A153562</v>
+        <v>A227197</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>A153564</v>
+        <v>A227200</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>A153565</v>
+        <v>A227201</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>A153566</v>
+        <v>A227203</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>A153567</v>
+        <v>A227202</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>A153574</v>
+        <v>A227210</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>A153575</v>
+        <v>A227209</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>A153578</v>
+        <v>A227214</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>A153579</v>
+        <v>A227213</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>A153582</v>
+        <v>A227215</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>A153583</v>
+        <v>A227219</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>A153584</v>
+        <v>A227218</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>A153585</v>
+        <v>A227220</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>A153586</v>
+        <v>A227223</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>A153588</v>
+        <v>A227224</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>A153589</v>
+        <v>A227225</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>A227227</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>A227226</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>A227228</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>A227229</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>A227230</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>A227231</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>A227235</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>A227236</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>A227237</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>A227240</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>A227241</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>A227242</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>A227245</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>A227246</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>A227247</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>A227251</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>A227252</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>A227253</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>A227257</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>A227256</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>A227258</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A48"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -634,60 +687,570 @@
         <v>Project ID</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>P-609807</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>P-609814</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>P-609815</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>P-609820</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>P-609829</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>DE-TIMS-100104</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>P-609832</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>P-609833</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>P-609836</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>P-609837</v>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>P-860180</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>P-860195</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>P-860208</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>P-860224</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>P-860233</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>P-860244</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>P-860253</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>P-860263</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>P-860306</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>P-860320</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>P-860334</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>P-860347</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>P-860360</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A26"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Request ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>R02083</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>R02084</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>R02085</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>R02086</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>R02088</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>R02089</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>R02090</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>R02095</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>R02096</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>R02097</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>R02098</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>R02102</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>R02103</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>R02104</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>R02108</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>R02109</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>R02114</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>R02115</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>R02116</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>R02117</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>R02125</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>R02126</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>R02131</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>R02136</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>R02137</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>R02138</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>R02143</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>R02148</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>R02149</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>R02150</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>R02155</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>R02156</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>R02161</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>R02162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A35"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Lease ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>ST-Lease-283252</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ST-Lease-283253</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ST-Lease-283254</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ST-Lease-283255</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>ST-Lease-283256</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>ST-Lease-283257</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>ST-Lease-283258</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ST-Lease-283259</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>ST-Lease-283264</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ST-Lease-283265</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>ST-Lease-283266</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>ST-Lease-283267</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>ST-Lease-283272</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>ST-Lease-283273</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>ST-Lease-283274</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>ST-Lease-283275</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>ST-Lease-283280</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>ST-Lease-283281</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>ST-Lease-283282</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>ST-Lease-283285</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>ST-Lease-283286</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>ST-Lease-283287</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>ST-Lease-283288</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>ST-Lease-283291</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>ST-Lease-283292</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>ST-Lease-283293</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>ST-Lease-283296</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>ST-Lease-283297</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>ST-Lease-283298</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>ST-Lease-283299</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>ST-Lease-283305</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>ST-Lease-283306</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>ST-Lease-283307</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>ST-Lease-283308</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>ST-Lease-283313</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>ST-Lease-283314</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>ST-Lease-283315</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>ST-Lease-283316</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>ST-Lease-283321</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>ST-Lease-283322</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>ST-Lease-283323</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>ST-Lease-283324</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>ST-Lease-283325</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>ST-Lease-283330</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>ST-Lease-283331</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>ST-Lease-283332</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>ST-Lease-283333</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>ST-Lease-283338</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>ST-Lease-283339</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>ST-Lease-283340</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>ST-Lease-283341</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>ST-Lease-283342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A53"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Candidate ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Auto test6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add sub-Project and Structure Equipment TCs
</commit_message>
<xml_diff>
--- a/createdRecords.xlsx
+++ b/createdRecords.xlsx
@@ -6,6 +6,15 @@
     <sheet name="Site" sheetId="1" r:id="rId1"/>
     <sheet name="Application" sheetId="2" r:id="rId2"/>
     <sheet name="Project" sheetId="3" r:id="rId3"/>
+    <sheet name="Requests" sheetId="4" r:id="rId4"/>
+    <sheet name="Leases" sheetId="5" r:id="rId5"/>
+    <sheet name="Candidates" sheetId="6" r:id="rId6"/>
+    <sheet name="SiteContacts" sheetId="7" r:id="rId7"/>
+    <sheet name="jobs" sheetId="8" r:id="rId8"/>
+    <sheet name="Site Access" sheetId="9" r:id="rId9"/>
+    <sheet name="Rental Object" sheetId="10" r:id="rId10"/>
+    <sheet name="External IDs" sheetId="11" r:id="rId11"/>
+    <sheet name="StructureEquipment" sheetId="12" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
@@ -472,9 +481,174 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Rental Object ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>RO-13671</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>RO-13672</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>RO-13675</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>RO-13692</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>RO-13694</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>RO-13695</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>RO-13696</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>RO-13697</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>RO-13698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>External IDs</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>EID-016033</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>EID-016054</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>EID-016055</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>EID-016056</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>EID-016089</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>EID-016090</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>EID-016091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A8"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>StructureEquipment ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>E-076148</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>E-076149</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>E-076150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>E-076151</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>E-076153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A86"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -614,15 +788,1185 @@
         <v>A153589</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>A153969</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>A153968</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>A153970</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>A153978</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>A153979</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>A153980</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>A153982</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>A153984</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>A153985</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>A153986</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>A153987</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>A153995</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>A153996</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>A153997</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>A153998</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>A153999</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>A154000</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>A154001</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>A154002</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>A154003</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>A154026</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>A154027</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>A154028</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>A154029</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>A154030</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>A154031</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>A154046</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>A154047</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>A154055</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>A154057</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>A154058</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>A154062</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>A154063</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>A154065</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>A154066</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>A154073</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>A154074</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>A154075</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>A154076</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>A154080</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>A154081</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>A154082</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>A154083</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>A154087</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>A154088</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>A154089</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>A154090</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>A154094</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>A154095</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>A154096</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>A154097</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>A154102</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>A154101</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>A154103</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>A154104</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>A154108</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>A154109</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>A154110</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>A154111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A86"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Project ID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>P-609807</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>P-609814</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>P-609815</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>P-609820</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>P-609829</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>DE-TIMS-100104</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>P-609832</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>P-609833</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>P-609836</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>P-609837</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>P-610592</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>P-732469</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>P-610619</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>P-610662</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>P-610692</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>P-610719</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>P-610743</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>P-610763</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>P-610786</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>P-610808</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>P-610829</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>P-610852</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A23"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>RequestID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>R00692</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>R00691</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>R00693</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>R00694</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>R00695</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>R00696</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>R00697</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>R00698</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>R00699</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>R00703</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>R00704</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>R00705</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>R00706</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>R00707</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>R00708</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>R00712</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>R00713</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>R00714</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>R00715</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>R00720</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>R00721</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>R00722</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>R00723</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>R00724</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>R00725</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>R00726</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>R00732</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>R00733</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>R00734</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>R00735</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>R00736</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>R00742</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>R00743</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>R00744</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>R00745</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>R00746</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>R00752</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>R00753</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>R00754</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>R00755</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>R00756</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>R00762</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>R00763</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>R00764</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>R00765</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>R00766</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>R00772</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>R00773</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>R00774</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>R00775</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>R00776</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>R00782</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>R00783</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>R00784</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>R00785</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>R00786</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A57"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>LeaseID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>ST-Lease-201227</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ST-Lease-201229</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ST-Lease-201232</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ST-Lease-201231</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>ST-Lease-201233</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>ST-Lease-201234</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>ST-Lease-201235</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ST-Lease-201236</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>ST-Lease-201237</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ST-Lease-201238</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>ST-Lease-201239</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>ST-Lease-201240</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>ST-Lease-201241</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>ST-Lease-201242</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>ST-Lease-201243</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>ST-Lease-201244</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>ST-Lease-201263</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>ST-Lease-201264</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>ST-Lease-201265</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>ST-Lease-201266</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>ST-Lease-201267</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>ST-Lease-201272</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>ST-Lease-201273</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>ST-Lease-201274</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>ST-Lease-201275</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>ST-Lease-201276</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>ST-Lease-201277</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>ST-Lease-201278</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>ST-Lease-201279</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>ST-Lease-201289</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>ST-Lease-201290</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>ST-Lease-201291</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>ST-Lease-201292</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>ST-Lease-201293</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>ST-Lease-201299</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>ST-Lease-201307</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>ST-Lease-201308</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>ST-Lease-201309</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>ST-Lease-201310</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>ST-Lease-201315</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>ST-Lease-201316</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>ST-Lease-201317</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>ST-Lease-201318</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>ST-Lease-201324</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>ST-Lease-201325</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>ST-Lease-201326</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>ST-Lease-201327</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>ST-Lease-201334</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>ST-Lease-201335</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>ST-Lease-201336</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>ST-Lease-201338</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>ST-Lease-201343</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>ST-Lease-201344</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>ST-Lease-201345</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>ST-Lease-201347</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>ST-Lease-201352</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>ST-Lease-201353</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>ST-Lease-201354</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>ST-Lease-201356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A60"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>candidateID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Auto test48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Auto test66</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Auto test2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Auto test46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Auto test62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>siteContactID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SC-0116978</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SC-0116980</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SC-0116982</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SC-0116985</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SC-0116987</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SC-0116989</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SC-0116990</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>SC-0116993</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>SC-0116994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>jobID</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -631,57 +1975,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Project ID</v>
+        <v>siteAccessID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>P-609807</v>
+        <v>REQ00338</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>P-609814</v>
+        <v>REQ00339</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>P-609815</v>
+        <v>REQ00341</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>P-609820</v>
+        <v>REQ00343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>P-609829</v>
+        <v>REQ00345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>DE-TIMS-100104</v>
+        <v>REQ00347</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>P-609832</v>
+        <v>REQ00349</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>P-609833</v>
+        <v>REQ00351</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>P-609836</v>
+        <v>REQ00353</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>P-609837</v>
+        <v>REQ00355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>